<commit_message>
add more functions related with QA solution
</commit_message>
<xml_diff>
--- a/QA list.xlsx
+++ b/QA list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitFolder\VMAT-QA-metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4213C1D-D03E-4824-BB41-FD046CF15610}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05991410-DCF2-4F9E-A640-993F26EF22D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{0FCD556E-0B02-4B5A-BF80-FF5679FDA974}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{0FCD556E-0B02-4B5A-BF80-FF5679FDA974}"/>
   </bookViews>
   <sheets>
     <sheet name="VMAT" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,8 +224,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,7 +266,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -267,6 +280,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -586,7 +608,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -648,7 +670,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B11" t="s">
@@ -656,22 +678,22 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add LSV_weighted & AAV_weighted
</commit_message>
<xml_diff>
--- a/QA list.xlsx
+++ b/QA list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitFolder\VMAT-QA-metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05991410-DCF2-4F9E-A640-993F26EF22D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A4D93A-A6B4-4D7D-B04F-DD376208DC83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{0FCD556E-0B02-4B5A-BF80-FF5679FDA974}"/>
+    <workbookView xWindow="-38235" yWindow="2085" windowWidth="18105" windowHeight="10320" xr2:uid="{0FCD556E-0B02-4B5A-BF80-FF5679FDA974}"/>
   </bookViews>
   <sheets>
     <sheet name="VMAT" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>Modulation index for total modulation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Standard deviation of leaf acceleration (SLA)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average leaf speed (ALS)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Proportion of leaf acceleration ranging</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -53,14 +41,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mean asymmetry distance (MAD)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modulation complexity score (MCS)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Leaf sequence variability (LSV)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -85,10 +65,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Union aperture area (UAA)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Edge metric (EM)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -105,10 +81,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Average leaf travel distance (LT)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Combination of LT and MCS (LTMCS)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -121,14 +93,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Average dose rate (ADR)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Standard deviation of dose rate (SDR)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>MU value in first arc (MU 1)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -160,31 +124,99 @@
     <t>QA metrics</t>
   </si>
   <si>
-    <t>formula</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modulation index for leaf speed (f=0.2,0.5,1,2)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modulation index for leaf acceleration (f=0.2,0.5,1,2)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Standard deviation of leaf speed (SLS)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average leaf acceleration (ALA)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Small aperture score (SAS)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>the proportion of open leaf pairs that were separated by less than a given threshold distance</t>
+    <t>Modulation index for leaf speed (f=0.2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf speed (f=0.5)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf speed (f=1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf speed (f=2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf acceleration (f=0.2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf acceleration (f=0.5)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf acceleration (f=1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for leaf acceleration (f=2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for total modulation(f=0.2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for total modulation(f=2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for total modulation(f=1)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modulation index for total modulation(f=0.5)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VMAT0028</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average leaf speed (ALS) mm/s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard deviation of leaf speed (SLS) mm/s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average leaf acceleration (ALA) mm/s^2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard deviation of leaf acceleration (SLA) mm/s^2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean asymmetry distance (MAD) mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulation complexity score (MCS) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Union aperture area (UAA) cm^2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average dose rate (ADR) MU/s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard deviation of dose rate (SDR) MU/s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average leaf travel distance (LT) mm</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -605,206 +637,342 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529A1111-B1BD-4F10-ADE9-DE8155E6DCC2}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>71.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>17.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>36.270000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>58.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B10">
+        <v>82.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B11">
+        <v>30.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>62.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>102.14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B14">
+        <v>143.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>10.39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>23.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>22.11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>35.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="B26">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="B27">
+        <v>9.89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="B28">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="B29">
+        <v>584.99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>421.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <v>325.32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B36">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>9.2200000000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B43">
+        <f>61.6/28</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates Small Aperture Score & Fix a bug for gantry speed
</commit_message>
<xml_diff>
--- a/QA list.xlsx
+++ b/QA list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitFolder\VMAT-QA-metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A4D93A-A6B4-4D7D-B04F-DD376208DC83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60C8B95-3842-464C-8EA1-388623C537EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38235" yWindow="2085" windowWidth="18105" windowHeight="10320" xr2:uid="{0FCD556E-0B02-4B5A-BF80-FF5679FDA974}"/>
+    <workbookView xWindow="-38520" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{0FCD556E-0B02-4B5A-BF80-FF5679FDA974}"/>
   </bookViews>
   <sheets>
     <sheet name="VMAT" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Proportion of leaf acceleration ranging</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>Average leaf travel distance (LT) mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VMAT0010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLC speed distribution</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Leaf Speed</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -637,29 +649,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529A1111-B1BD-4F10-ADE9-DE8155E6DCC2}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -667,7 +683,7 @@
         <v>15.74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -675,7 +691,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -683,7 +699,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -691,7 +707,7 @@
         <v>71.23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -699,7 +715,7 @@
         <v>17.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -707,7 +723,7 @@
         <v>36.270000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -715,7 +731,7 @@
         <v>58.66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -723,7 +739,7 @@
         <v>82.33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -731,7 +747,7 @@
         <v>30.22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -739,7 +755,7 @@
         <v>62.99</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -747,7 +763,7 @@
         <v>102.14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -755,12 +771,12 @@
         <v>143.26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -973,6 +989,16 @@
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>